<commit_message>
All cases resolved, ready to show.
</commit_message>
<xml_diff>
--- a/Code/Limpio/Excels/modelo MM - TALCA 28.12_v5.xlsx
+++ b/Code/Limpio/Excels/modelo MM - TALCA 28.12_v5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\6020.Inecon_ModeloVanMedicion\6020.Inecon_ModeloVanMedicion\Code\Limpio\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22ADA04-30EF-4BAA-A592-7C5272A006D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7B339E-9A89-4764-8894-757AB03C968D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="6" xr2:uid="{0B67A8E0-BE2B-4F48-8F89-95A6B35879D7}"/>
   </bookViews>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="344">
   <si>
     <t>Intervalo (l/h)</t>
   </si>
@@ -1153,6 +1153,9 @@
   </si>
   <si>
     <t>Para cálculo de impuesto</t>
+  </si>
+  <si>
+    <t>OJALAIGNOREESTA</t>
   </si>
 </sst>
 </file>
@@ -24785,7 +24788,7 @@
   <dimension ref="A1:N169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25225,16 +25228,36 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="42"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
+      <c r="A11" s="42">
+        <v>45138</v>
+      </c>
+      <c r="B11" s="156" t="s">
+        <v>343</v>
+      </c>
+      <c r="C11" s="38">
+        <v>1.255E-2</v>
+      </c>
+      <c r="D11" s="39">
+        <v>0</v>
+      </c>
+      <c r="E11" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="31">
+        <v>15</v>
+      </c>
+      <c r="H11" s="31">
+        <v>0</v>
+      </c>
+      <c r="I11" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="31">
+        <v>4.5</v>
+      </c>
       <c r="K11" s="32"/>
       <c r="M11" s="26"/>
       <c r="N11" s="32"/>
@@ -27618,9 +27641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F3A346-95CC-40C7-A048-A8DCA15A773E}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I10"/>
-    </sheetView>
+    <sheetView topLeftCell="A40" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -29774,11 +29795,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="afef9374-bd24-49fe-b5be-cd056ccbd7a9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29970,26 +29992,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="afef9374-bd24-49fe-b5be-cd056ccbd7a9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F368767-011F-4603-B6D3-67B09FEB0E3E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{799D9F8D-2034-4116-9680-A411761E28F5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="afef9374-bd24-49fe-b5be-cd056ccbd7a9"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -30013,9 +30026,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{799D9F8D-2034-4116-9680-A411761E28F5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F368767-011F-4603-B6D3-67B09FEB0E3E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="afef9374-bd24-49fe-b5be-cd056ccbd7a9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>